<commit_message>
revisions to metadata and documentation
</commit_message>
<xml_diff>
--- a/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
+++ b/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-growth-grazing-chl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6F68EA-C727-8749-8201-A9CFBEE85C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B4FEB-8D44-A84F-BABB-6F16450A1EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25660" yWindow="460" windowWidth="33320" windowHeight="19100" activeTab="1" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="314">
   <si>
     <t>givenName</t>
   </si>
@@ -1206,9 +1206,6 @@
     <t>Not determined because g &lt; 0, which is a violation of dilution method's assumption. </t>
   </si>
   <si>
-    <t xml:space="preserve">Not available because no Chl-a size fractionnation was performed. </t>
-  </si>
-  <si>
     <t>Not nutrient limited, thus no value.</t>
   </si>
   <si>
@@ -1336,6 +1333,27 @@
   </si>
   <si>
     <t>celsius</t>
+  </si>
+  <si>
+    <t>Date and time of sampling (UTC). The value given here is the mean value for multiple Niskin bottle closure where the seawater sample comes from</t>
+  </si>
+  <si>
+    <t>Uncertainty relative to µ0 estimated from the standard deviation observed on the apparent phytoplankton growth rate kNoN in nutrient unamended treatment (see associated computation methods)</t>
+  </si>
+  <si>
+    <t>Uncertainty relative to µN estimated from the standard deviation observed on the apparent phytoplankton growth rate kN in nutrient amended treatment (see associated computation methods)</t>
+  </si>
+  <si>
+    <t>Uncertainty relative to µ Chl-a &lt; 10 µm estimated from the standard deviation observed on the apparent phytoplankton growth rate k computed from Chl-a &lt;10µm.</t>
+  </si>
+  <si>
+    <t>Uncertainty relative to µ Chl-a &gt; 10 µm estimated from the standard deviation observed on the apparent phytoplankton growth rate k computed from Chl-a &gt;10µm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not available because no Chl-a size fractionation was performed. </t>
+  </si>
+  <si>
+    <t>PSU</t>
   </si>
 </sst>
 </file>
@@ -4893,8 +4911,8 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -4967,14 +4985,14 @@
         <v>173</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>219</v>
+        <v>307</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
@@ -4999,7 +5017,7 @@
         <v>166</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>208</v>
@@ -5014,7 +5032,7 @@
         <v>167</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>208</v>
@@ -5035,7 +5053,7 @@
         <v>210</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
@@ -5052,7 +5070,7 @@
         <v>210</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -5069,7 +5087,7 @@
         <v>210</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -5086,7 +5104,7 @@
         <v>210</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -5103,7 +5121,7 @@
         <v>210</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>211</v>
+        <v>313</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -5117,11 +5135,11 @@
         <v>230</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
@@ -5134,11 +5152,11 @@
         <v>231</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
@@ -5148,7 +5166,7 @@
         <v>176</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>210</v>
@@ -5182,7 +5200,7 @@
         <v>111</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>196</v>
+        <v>308</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>210</v>
@@ -5199,7 +5217,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>210</v>
@@ -5212,18 +5230,18 @@
         <v>-9999</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16">
       <c r="A19" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>292</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>293</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -5235,7 +5253,7 @@
         <v>112</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>197</v>
+        <v>309</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>210</v>
@@ -5248,18 +5266,18 @@
         <v>-9999</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16">
       <c r="A21" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -5271,7 +5289,7 @@
         <v>179</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>210</v>
@@ -5284,18 +5302,18 @@
         <v>-9999</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16">
       <c r="A23" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -5307,7 +5325,7 @@
         <v>180</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>210</v>
@@ -5320,18 +5338,18 @@
         <v>-9999</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16">
       <c r="A25" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -5343,7 +5361,7 @@
         <v>116</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>210</v>
@@ -5356,18 +5374,18 @@
         <v>-9999</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16">
       <c r="A27" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -5379,7 +5397,7 @@
         <v>117</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>204</v>
+        <v>310</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>210</v>
@@ -5392,18 +5410,18 @@
         <v>-9999</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16">
       <c r="A29" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -5428,18 +5446,18 @@
         <v>-9999</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16">
       <c r="A31" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -5464,18 +5482,18 @@
         <v>-9999</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16">
       <c r="A33" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -5487,7 +5505,7 @@
         <v>114</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>210</v>
@@ -5500,18 +5518,18 @@
         <v>-9999</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16">
       <c r="A35" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -5523,7 +5541,7 @@
         <v>115</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>205</v>
+        <v>311</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>210</v>
@@ -5536,18 +5554,18 @@
         <v>-9999</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16">
       <c r="A37" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -5572,18 +5590,18 @@
         <v>-9999</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16">
       <c r="A39" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -5608,18 +5626,18 @@
         <v>-9999</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16">
       <c r="A41" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -6278,7 +6296,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B3" t="s">
         <v>244</v>
@@ -6289,7 +6307,7 @@
         <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6297,65 +6315,65 @@
         <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6618,40 +6636,40 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>113</v>
@@ -6662,7 +6680,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>113</v>
@@ -6673,51 +6691,51 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>113</v>
@@ -6728,29 +6746,29 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>113</v>
@@ -6761,51 +6779,51 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>113</v>
@@ -6816,18 +6834,18 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>113</v>
@@ -6838,13 +6856,13 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisions to methods, custom units, and parent project
</commit_message>
<xml_diff>
--- a/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
+++ b/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-growth-grazing-chl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B4FEB-8D44-A84F-BABB-6F16450A1EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33D6F79-3B67-2D40-856C-DC3712283DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25660" yWindow="460" windowWidth="33320" windowHeight="19100" activeTab="1" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="4" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="317">
   <si>
     <t>givenName</t>
   </si>
@@ -1354,6 +1354,15 @@
   </si>
   <si>
     <t>PSU</t>
+  </si>
+  <si>
+    <t>practical salinity unit</t>
+  </si>
+  <si>
+    <t>gramsPerKilogram</t>
+  </si>
+  <si>
+    <t>massPerUnitVolume</t>
   </si>
 </sst>
 </file>
@@ -4910,9 +4919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7951F9-6AD5-1A4E-A353-6C10A708B787}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -5178,7 +5187,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" ht="40" customHeight="1">
+    <row r="16" spans="1:7" ht="54" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>24</v>
       </c>
@@ -6388,16 +6397,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CDE20D-D78A-F942-8FF6-0BCBED7BA37D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6433,6 +6443,23 @@
       </c>
       <c r="E2" t="s">
         <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
retracted changes to custom units
</commit_message>
<xml_diff>
--- a/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
+++ b/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-growth-grazing-chl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33D6F79-3B67-2D40-856C-DC3712283DC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77429172-9E01-044A-A6C3-F8DCC063D660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="4" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
+    <workbookView xWindow="32600" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="4" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="314">
   <si>
     <t>givenName</t>
   </si>
@@ -1353,16 +1353,7 @@
     <t xml:space="preserve">Not available because no Chl-a size fractionation was performed. </t>
   </si>
   <si>
-    <t>PSU</t>
-  </si>
-  <si>
-    <t>practical salinity unit</t>
-  </si>
-  <si>
-    <t>gramsPerKilogram</t>
-  </si>
-  <si>
-    <t>massPerUnitVolume</t>
+    <t>Salinity of sampling. The value given here is the mean salinity in PSU at which each bottle was fired</t>
   </si>
 </sst>
 </file>
@@ -4920,8 +4911,8 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -5124,13 +5115,13 @@
         <v>172</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>193</v>
+        <v>313</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>313</v>
+        <v>211</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -6397,10 +6388,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CDE20D-D78A-F942-8FF6-0BCBED7BA37D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6443,23 +6434,6 @@
       </c>
       <c r="E2" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>313</v>
-      </c>
-      <c r="B3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C3" t="s">
-        <v>315</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to custom units
</commit_message>
<xml_diff>
--- a/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
+++ b/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-growth-grazing-chl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77429172-9E01-044A-A6C3-F8DCC063D660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F385259-9307-B94B-9454-6997740338D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32600" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="4" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
+    <workbookView xWindow="26560" yWindow="460" windowWidth="27380" windowHeight="18500" activeTab="1" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1167,18 +1168,12 @@
     <t>keyword</t>
   </si>
   <si>
-    <t>number per day</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>rate</t>
   </si>
   <si>
-    <t>numberPerDay</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -1354,6 +1349,12 @@
   </si>
   <si>
     <t>Salinity of sampling. The value given here is the mean salinity in PSU at which each bottle was fired</t>
+  </si>
+  <si>
+    <t>perDay</t>
+  </si>
+  <si>
+    <t>per day</t>
   </si>
 </sst>
 </file>
@@ -4910,9 +4911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7951F9-6AD5-1A4E-A353-6C10A708B787}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -4985,14 +4986,14 @@
         <v>173</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
@@ -5017,7 +5018,7 @@
         <v>166</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>208</v>
@@ -5032,7 +5033,7 @@
         <v>167</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>208</v>
@@ -5053,7 +5054,7 @@
         <v>210</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
@@ -5070,7 +5071,7 @@
         <v>210</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -5087,7 +5088,7 @@
         <v>210</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -5104,7 +5105,7 @@
         <v>210</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -5115,7 +5116,7 @@
         <v>172</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>210</v>
@@ -5135,11 +5136,11 @@
         <v>230</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
@@ -5152,11 +5153,11 @@
         <v>231</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
@@ -5166,7 +5167,7 @@
         <v>176</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>210</v>
@@ -5189,7 +5190,7 @@
         <v>210</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -5200,13 +5201,13 @@
         <v>111</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
@@ -5217,31 +5218,31 @@
         <v>25</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16">
         <v>-9999</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16">
       <c r="A19" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>293</v>
-      </c>
       <c r="C19" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -5253,31 +5254,31 @@
         <v>112</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16">
         <v>-9999</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16">
       <c r="A21" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -5289,31 +5290,31 @@
         <v>179</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16">
         <v>-9999</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16">
       <c r="A23" s="18" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -5325,31 +5326,31 @@
         <v>180</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16">
         <v>-9999</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16">
       <c r="A25" s="18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -5361,31 +5362,31 @@
         <v>116</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16">
         <v>-9999</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16">
       <c r="A27" s="18" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -5397,31 +5398,31 @@
         <v>117</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16">
         <v>-9999</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16">
       <c r="A29" s="18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -5439,25 +5440,25 @@
         <v>210</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16">
         <v>-9999</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16">
       <c r="A31" s="18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -5475,25 +5476,25 @@
         <v>210</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E32" s="16"/>
       <c r="F32" s="16">
         <v>-9999</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16">
       <c r="A33" s="18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -5505,31 +5506,31 @@
         <v>114</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="16">
         <v>-9999</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16">
       <c r="A35" s="18" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -5541,31 +5542,31 @@
         <v>115</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16">
         <v>-9999</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16">
       <c r="A37" s="18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -5583,25 +5584,25 @@
         <v>210</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="16">
         <v>-9999</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16">
       <c r="A39" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -5619,25 +5620,25 @@
         <v>210</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="E40" s="16"/>
       <c r="F40" s="16">
         <v>-9999</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16">
       <c r="A41" s="18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -6296,7 +6297,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s">
         <v>244</v>
@@ -6307,7 +6308,7 @@
         <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6315,65 +6316,65 @@
         <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6390,8 +6391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CDE20D-D78A-F942-8FF6-0BCBED7BA37D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6404,36 +6405,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>251</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -6446,7 +6447,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6509,7 +6510,7 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -6538,7 +6539,7 @@
         <v>234</v>
       </c>
       <c r="F3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G3" t="s">
         <v>235</v>
@@ -6593,7 +6594,7 @@
         <v>242</v>
       </c>
       <c r="F5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G5" t="s">
         <v>243</v>
@@ -6637,233 +6638,233 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove local edi-utilities and fix various errors
</commit_message>
<xml_diff>
--- a/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
+++ b/NES-LTER_Growth-Grazing_SMD_2019_11_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-growth-grazing-chl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkoch\Desktop\LTER\nes-lter-growth-grazing-chl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F385259-9307-B94B-9454-6997740338D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F394BE-E40F-4DFE-A24F-DD371A97D0A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26560" yWindow="460" windowWidth="27380" windowHeight="18500" activeTab="1" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
+    <workbookView xWindow="26562" yWindow="462" windowWidth="27378" windowHeight="18498" activeTab="6" xr2:uid="{9B5322E1-0235-42A2-BB26-F491C21C6910}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="1" r:id="rId1"/>
@@ -26,18 +26,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="313">
   <si>
     <t>givenName</t>
   </si>
@@ -1204,15 +1198,9 @@
     <t>Not nutrient limited, thus no value.</t>
   </si>
   <si>
-    <t>Definition</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
-    <t>attribute</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -1355,6 +1343,9 @@
   </si>
   <si>
     <t>per day</t>
+  </si>
+  <si>
+    <t>definition</t>
   </si>
 </sst>
 </file>
@@ -1818,37 +1809,37 @@
       <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="2"/>
-    <col min="2" max="2" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="2"/>
+    <col min="2" max="2" width="6.47265625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.3125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.68359375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.3125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.47265625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.47265625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.3125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.15625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.47265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.47265625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.68359375" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.1640625" style="2"/>
+    <col min="26" max="26" width="11.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="35.83984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -4911,24 +4902,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7951F9-6AD5-1A4E-A353-6C10A708B787}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+    <sheetView zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="15"/>
+    <col min="1" max="1" width="13.68359375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="43.15625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="9.15625" style="15"/>
     <col min="4" max="4" width="14" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.1640625" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="15"/>
+    <col min="5" max="5" width="17.83984375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="17.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.15625" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="9.15625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:7">
       <c r="A1" s="16" t="s">
         <v>139</v>
       </c>
@@ -4951,7 +4942,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16">
+    <row r="2" spans="1:7">
       <c r="A2" s="18" t="s">
         <v>163</v>
       </c>
@@ -4966,7 +4957,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="1:7" ht="16">
+    <row r="3" spans="1:7">
       <c r="A3" s="18" t="s">
         <v>164</v>
       </c>
@@ -4981,24 +4972,24 @@
       <c r="F3" s="16"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" ht="48">
+    <row r="4" spans="1:7" ht="55.2">
       <c r="A4" s="19" t="s">
         <v>173</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" ht="32">
+    <row r="5" spans="1:7" ht="27.6">
       <c r="A5" s="18" t="s">
         <v>165</v>
       </c>
@@ -5018,7 +5009,7 @@
         <v>166</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>208</v>
@@ -5033,7 +5024,7 @@
         <v>167</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>208</v>
@@ -5043,7 +5034,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:7" ht="32">
+    <row r="8" spans="1:7" ht="27.6">
       <c r="A8" s="18" t="s">
         <v>168</v>
       </c>
@@ -5054,13 +5045,13 @@
         <v>210</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" ht="32">
+    <row r="9" spans="1:7" ht="41.4">
       <c r="A9" s="18" t="s">
         <v>169</v>
       </c>
@@ -5071,13 +5062,13 @@
         <v>210</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" ht="32">
+    <row r="10" spans="1:7" ht="27.6">
       <c r="A10" s="18" t="s">
         <v>170</v>
       </c>
@@ -5088,13 +5079,13 @@
         <v>210</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" ht="32">
+    <row r="11" spans="1:7" ht="41.4">
       <c r="A11" s="18" t="s">
         <v>171</v>
       </c>
@@ -5105,18 +5096,18 @@
         <v>210</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" ht="32">
+    <row r="12" spans="1:7" ht="41.4">
       <c r="A12" s="18" t="s">
         <v>172</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>210</v>
@@ -5128,7 +5119,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" ht="16">
+    <row r="13" spans="1:7" ht="27.6">
       <c r="A13" s="18" t="s">
         <v>174</v>
       </c>
@@ -5136,16 +5127,16 @@
         <v>230</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" ht="16">
+    <row r="14" spans="1:7">
       <c r="A14" s="18" t="s">
         <v>175</v>
       </c>
@@ -5153,21 +5144,21 @@
         <v>231</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="32">
+    <row r="15" spans="1:7" ht="27.6">
       <c r="A15" s="18" t="s">
         <v>176</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>210</v>
@@ -5190,246 +5181,246 @@
         <v>210</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="64">
+    <row r="17" spans="1:7" ht="69">
       <c r="A17" s="18" t="s">
         <v>111</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="64">
+    <row r="18" spans="1:7" ht="69">
       <c r="A18" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16">
         <v>-9999</v>
       </c>
       <c r="G18" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="16">
-      <c r="A19" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="64">
+    <row r="20" spans="1:7" ht="69">
       <c r="A20" s="18" t="s">
         <v>112</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16">
         <v>-9999</v>
       </c>
       <c r="G20" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="16">
-      <c r="A21" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="32">
+    <row r="22" spans="1:7" ht="27.6">
       <c r="A22" s="18" t="s">
         <v>179</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16">
         <v>-9999</v>
       </c>
       <c r="G22" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C23" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16">
-      <c r="A23" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="48">
+    <row r="24" spans="1:7" ht="55.2">
       <c r="A24" s="18" t="s">
         <v>180</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16">
         <v>-9999</v>
       </c>
       <c r="G24" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="16">
-      <c r="A25" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" ht="64">
+    <row r="26" spans="1:7" ht="55.2">
       <c r="A26" s="18" t="s">
         <v>116</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16">
         <v>-9999</v>
       </c>
       <c r="G26" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="16">
-      <c r="A27" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="17"/>
     </row>
-    <row r="28" spans="1:7" ht="64">
+    <row r="28" spans="1:7" ht="55.2">
       <c r="A28" s="18" t="s">
         <v>117</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16">
         <v>-9999</v>
       </c>
       <c r="G28" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C29" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="16">
-      <c r="A29" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
     </row>
-    <row r="30" spans="1:7" ht="32">
+    <row r="30" spans="1:7" ht="27.6">
       <c r="A30" s="18" t="s">
         <v>177</v>
       </c>
@@ -5440,32 +5431,32 @@
         <v>210</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16">
         <v>-9999</v>
       </c>
       <c r="G30" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="16">
-      <c r="A31" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
       <c r="G31" s="17"/>
     </row>
-    <row r="32" spans="1:7" ht="48">
+    <row r="32" spans="1:7" ht="55.2">
       <c r="A32" s="18" t="s">
         <v>178</v>
       </c>
@@ -5476,104 +5467,104 @@
         <v>210</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E32" s="16"/>
       <c r="F32" s="16">
         <v>-9999</v>
       </c>
       <c r="G32" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="16">
-      <c r="A33" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
       <c r="G33" s="17"/>
     </row>
-    <row r="34" spans="1:7" ht="32">
+    <row r="34" spans="1:7" ht="27.6">
       <c r="A34" s="18" t="s">
         <v>114</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="16">
         <v>-9999</v>
       </c>
       <c r="G34" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="16">
-      <c r="A35" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="17"/>
     </row>
-    <row r="36" spans="1:7" ht="64">
+    <row r="36" spans="1:7" ht="55.2">
       <c r="A36" s="18" t="s">
         <v>115</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>210</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16">
         <v>-9999</v>
       </c>
       <c r="G36" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="16">
-      <c r="A37" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" ht="32">
+    <row r="38" spans="1:7" ht="27.6">
       <c r="A38" s="18" t="s">
         <v>181</v>
       </c>
@@ -5584,32 +5575,32 @@
         <v>210</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="16">
         <v>-9999</v>
       </c>
       <c r="G38" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="16">
-      <c r="A39" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" ht="48">
+    <row r="40" spans="1:7" ht="55.2">
       <c r="A40" s="18" t="s">
         <v>182</v>
       </c>
@@ -5620,32 +5611,32 @@
         <v>210</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E40" s="16"/>
       <c r="F40" s="16">
         <v>-9999</v>
       </c>
       <c r="G40" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="C41" s="16" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="16">
-      <c r="A41" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>290</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="17"/>
     </row>
-    <row r="42" spans="1:7" ht="160">
+    <row r="42" spans="1:7" ht="165.6">
       <c r="A42" s="19" t="s">
         <v>183</v>
       </c>
@@ -5674,20 +5665,20 @@
       <selection activeCell="G18" sqref="G18:G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.5" style="15" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="15"/>
+    <col min="1" max="1" width="22.3125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.47265625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9.15625" style="15"/>
     <col min="5" max="5" width="14" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.1640625" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="15"/>
+    <col min="6" max="6" width="29.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.15625" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="9.15625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16">
+    <row r="1" spans="1:8">
       <c r="A1" s="15" t="s">
         <v>138</v>
       </c>
@@ -5713,7 +5704,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16">
+    <row r="2" spans="1:8">
       <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
@@ -5727,7 +5718,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16">
+    <row r="3" spans="1:8">
       <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
@@ -5741,7 +5732,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32">
+    <row r="4" spans="1:8" ht="28.8">
       <c r="A4" s="13" t="s">
         <v>31</v>
       </c>
@@ -5758,7 +5749,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16">
+    <row r="5" spans="1:8">
       <c r="A5" s="11" t="s">
         <v>30</v>
       </c>
@@ -5772,7 +5763,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="32">
+    <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
@@ -5789,7 +5780,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="64">
+    <row r="7" spans="1:8" ht="57.6">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -5806,7 +5797,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17">
+    <row r="8" spans="1:8" ht="16.5">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
@@ -5823,7 +5814,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17">
+    <row r="9" spans="1:8" ht="16.5">
       <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
@@ -5840,7 +5831,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16">
+    <row r="10" spans="1:8">
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
@@ -5857,7 +5848,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17">
+    <row r="11" spans="1:8" ht="28.8">
       <c r="A11" s="11" t="s">
         <v>162</v>
       </c>
@@ -5874,7 +5865,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16">
+    <row r="12" spans="1:8">
       <c r="A12" s="11" t="s">
         <v>161</v>
       </c>
@@ -5891,7 +5882,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16">
+    <row r="13" spans="1:8">
       <c r="A13" s="11"/>
       <c r="B13" s="11" t="s">
         <v>174</v>
@@ -5906,7 +5897,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16">
+    <row r="14" spans="1:8">
       <c r="A14" s="11"/>
       <c r="B14" s="11" t="s">
         <v>175</v>
@@ -5921,7 +5912,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16">
+    <row r="15" spans="1:8">
       <c r="A15" s="11" t="s">
         <v>160</v>
       </c>
@@ -5938,7 +5929,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="32">
+    <row r="16" spans="1:8" ht="28.8">
       <c r="A16" s="11" t="s">
         <v>146</v>
       </c>
@@ -5955,7 +5946,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="48">
+    <row r="17" spans="1:8" ht="43.2">
       <c r="A17" s="11" t="s">
         <v>147</v>
       </c>
@@ -5972,7 +5963,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="48">
+    <row r="18" spans="1:8" ht="43.2">
       <c r="A18" s="11" t="s">
         <v>148</v>
       </c>
@@ -5995,7 +5986,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="32">
+    <row r="19" spans="1:8" ht="28.8">
       <c r="A19" s="11" t="s">
         <v>149</v>
       </c>
@@ -6018,7 +6009,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="32">
+    <row r="20" spans="1:8" ht="28.8">
       <c r="A20" s="11" t="s">
         <v>150</v>
       </c>
@@ -6041,7 +6032,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="32">
+    <row r="21" spans="1:8" ht="28.8">
       <c r="A21" s="11" t="s">
         <v>151</v>
       </c>
@@ -6064,7 +6055,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="48">
+    <row r="22" spans="1:8" ht="43.2">
       <c r="A22" s="11" t="s">
         <v>152</v>
       </c>
@@ -6087,7 +6078,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="48">
+    <row r="23" spans="1:8" ht="43.2">
       <c r="A23" s="11" t="s">
         <v>153</v>
       </c>
@@ -6110,7 +6101,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="64">
+    <row r="24" spans="1:8" ht="57.6">
       <c r="A24" s="11" t="s">
         <v>154</v>
       </c>
@@ -6133,7 +6124,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="64">
+    <row r="25" spans="1:8" ht="57.6">
       <c r="A25" s="11" t="s">
         <v>155</v>
       </c>
@@ -6156,7 +6147,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17">
+    <row r="26" spans="1:8" ht="16.5">
       <c r="A26" s="11" t="s">
         <v>156</v>
       </c>
@@ -6179,7 +6170,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="32">
+    <row r="27" spans="1:8" ht="28.8">
       <c r="A27" s="11" t="s">
         <v>157</v>
       </c>
@@ -6202,7 +6193,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="48">
+    <row r="28" spans="1:8" ht="43.2">
       <c r="A28" s="11" t="s">
         <v>158</v>
       </c>
@@ -6225,7 +6216,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="48">
+    <row r="29" spans="1:8" ht="43.2">
       <c r="A29" s="11" t="s">
         <v>159</v>
       </c>
@@ -6248,7 +6239,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="80">
+    <row r="30" spans="1:8" ht="86.4">
       <c r="A30" s="13"/>
       <c r="B30" s="13" t="s">
         <v>183</v>
@@ -6274,7 +6265,7 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
@@ -6297,7 +6288,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
         <v>244</v>
@@ -6308,7 +6299,7 @@
         <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6316,65 +6307,65 @@
         <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6395,12 +6386,12 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6422,7 +6413,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B2" t="s">
         <v>252</v>
@@ -6434,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -6450,18 +6441,18 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.15625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.47265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.47265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.47265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -6627,29 +6618,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACBB153-E9E4-4746-B6B2-F655753C5701}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>265</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1" t="s">
-        <v>263</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>120</v>
@@ -6660,7 +6651,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>120</v>
@@ -6671,7 +6662,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>113</v>
@@ -6682,7 +6673,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>113</v>
@@ -6693,51 +6684,51 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>113</v>
@@ -6748,29 +6739,29 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>113</v>
@@ -6781,51 +6772,51 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>113</v>
@@ -6836,18 +6827,18 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>113</v>
@@ -6858,13 +6849,13 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>